<commit_message>
Previous task has been fixed, Smoke Test task was added
</commit_message>
<xml_diff>
--- a/Mobile Testing/MobileTesting.xlsx
+++ b/Mobile Testing/MobileTesting.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A7F0D8F-3B3E-4CF8-B98C-05F316E3608D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DBA02C74-1551-47A5-B261-AC11B088003F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,13 +41,6 @@
     <t>Preconditions</t>
   </si>
   <si>
-    <t xml:space="preserve">Honor 7x
-Android version 8.0.0 
-RAM 4 GB 
-CPU Kirin 659
-</t>
-  </si>
-  <si>
     <t xml:space="preserve">Environment </t>
   </si>
   <si>
@@ -220,13 +213,6 @@
 2. Tap on "Miso soup" picture</t>
   </si>
   <si>
-    <t>Apple device:
-Tablet Apple iPad 9.7 Wi-Fi 32GB
-OS: iOS 12.0
-Browser: Safari
-Version: 12.0</t>
-  </si>
-  <si>
     <t>Orientation: Landscape</t>
   </si>
   <si>
@@ -275,6 +261,23 @@
 3. User type valid information to pop-up massage 
 4. User fills captcha
 5. User click on "Make a complain" button
+</t>
+  </si>
+  <si>
+    <t>Apple device:
+Tablet Apple iPad 
+Screen:9.7", 2048x1536
+Wi-Fi 32GB
+OS: iOS 12.0
+Browser: Safari
+Version: 12.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Honor 7x
+Screen: 5,93" , 2160x1080
+Android version 8.0.0 
+RAM 4 GB 
+CPU Kirin 659
 </t>
   </si>
 </sst>
@@ -421,6 +424,12 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -430,20 +439,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -735,7 +738,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -746,7 +749,7 @@
     <col min="4" max="4" width="45.85546875" customWidth="1"/>
     <col min="5" max="5" width="66.140625" customWidth="1"/>
     <col min="6" max="6" width="45.7109375" customWidth="1"/>
-    <col min="7" max="7" width="22.5703125" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -769,7 +772,7 @@
         <v>3</v>
       </c>
       <c r="G1" s="12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -777,22 +780,22 @@
         <v>1</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="13" t="s">
-        <v>6</v>
+      <c r="G2" s="15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="123.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -800,189 +803,189 @@
         <v>2</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="14"/>
+      <c r="G3" s="16"/>
     </row>
     <row r="4" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="14"/>
+        <v>14</v>
+      </c>
+      <c r="G4" s="16"/>
     </row>
     <row r="5" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+        <v>15</v>
+      </c>
+      <c r="G5" s="16"/>
+    </row>
+    <row r="6" spans="1:7" ht="135" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G6" s="14"/>
-    </row>
-    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="G6" s="16"/>
+    </row>
+    <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="G7" s="14"/>
+        <v>23</v>
+      </c>
+      <c r="G7" s="16"/>
     </row>
     <row r="8" spans="1:7" ht="120" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="F8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="G8" s="14"/>
+      <c r="G8" s="16"/>
     </row>
     <row r="9" spans="1:7" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="F9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="14"/>
-    </row>
-    <row r="10" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="G9" s="16"/>
+    </row>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="F10" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="G10" s="14"/>
+      <c r="G10" s="16"/>
     </row>
     <row r="11" spans="1:7" ht="75" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="G11" s="15"/>
+      <c r="G11" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -998,7 +1001,7 @@
   <dimension ref="A1:J13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1008,7 +1011,7 @@
     <col min="4" max="4" width="39.7109375" customWidth="1"/>
     <col min="5" max="5" width="32.28515625" customWidth="1"/>
     <col min="6" max="6" width="39.42578125" customWidth="1"/>
-    <col min="7" max="7" width="23.28515625" customWidth="1"/>
+    <col min="7" max="7" width="28.42578125" customWidth="1"/>
     <col min="8" max="8" width="24.42578125" customWidth="1"/>
     <col min="9" max="9" width="27.5703125" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
@@ -1019,29 +1022,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="H1" s="16" t="s">
-        <v>39</v>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1049,25 +1052,25 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="E2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -1075,23 +1078,23 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E3" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>50</v>
       </c>
       <c r="G3" s="19"/>
       <c r="H3" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="90" x14ac:dyDescent="0.25">
@@ -1099,23 +1102,23 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="F4" s="17" t="s">
-        <v>54</v>
+      <c r="F4" s="14" t="s">
+        <v>52</v>
       </c>
       <c r="G4" s="19"/>
       <c r="H4" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="150" x14ac:dyDescent="0.25">
@@ -1123,28 +1126,28 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D5" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>58</v>
-      </c>
       <c r="F5" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="J7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>